<commit_message>
bug fix/ with respect to schema
</commit_message>
<xml_diff>
--- a/SampleInputFiles/Test.xlsx
+++ b/SampleInputFiles/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishn\OneDrive\Desktop\MyEngineering\golocalrefactor\SampleInputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B20ADCD-2458-4881-9B50-5BDA2BA9AEF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E22505E-61BF-4F83-95D1-76165C4188F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="0" windowWidth="23040" windowHeight="9000" tabRatio="896" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12133" yWindow="0" windowWidth="23040" windowHeight="9000" tabRatio="896" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="100" r:id="rId1"/>
@@ -2007,8 +2007,8 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2925,7 +2925,7 @@
   </sheetPr>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection sqref="A1:G33"/>
     </sheetView>
   </sheetViews>
@@ -16305,6 +16305,27 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Project xmlns="a059ad7d-a67f-441f-a04d-fea35a8d4805" xsi:nil="true"/>
+    <Hashtags xmlns="a059ad7d-a67f-441f-a04d-fea35a8d4805"/>
+    <AppliedHashtags xmlns="b1b2b231-6a9c-427e-b130-2bce2f1f8dc6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100797130D9C3C45341B7E434CCDBD00C3A" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="96f1c79b8131947133353ad03edf7743">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="b1b2b231-6a9c-427e-b130-2bce2f1f8dc6" xmlns:ns3="d173ed03-a843-4ceb-a512-f7ef0c28f5c6" xmlns:ns4="a059ad7d-a67f-441f-a04d-fea35a8d4805" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="683ab32aecd624e993fbcfd4a3d9d029" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16566,27 +16587,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Project xmlns="a059ad7d-a67f-441f-a04d-fea35a8d4805" xsi:nil="true"/>
-    <Hashtags xmlns="a059ad7d-a67f-441f-a04d-fea35a8d4805"/>
-    <AppliedHashtags xmlns="b1b2b231-6a9c-427e-b130-2bce2f1f8dc6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84073E95-7368-461D-8739-B9D088CF2656}">
   <ds:schemaRefs>
@@ -16596,22 +16596,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D132EB-74DE-4A00-8207-CAF849BAD13A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369A900B-2FA8-4EC7-80F7-B143E0C8CFE2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="b1b2b231-6a9c-427e-b130-2bce2f1f8dc6"/>
-    <ds:schemaRef ds:uri="d173ed03-a843-4ceb-a512-f7ef0c28f5c6"/>
-    <ds:schemaRef ds:uri="a059ad7d-a67f-441f-a04d-fea35a8d4805"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16636,9 +16623,22 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369A900B-2FA8-4EC7-80F7-B143E0C8CFE2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D132EB-74DE-4A00-8207-CAF849BAD13A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="b1b2b231-6a9c-427e-b130-2bce2f1f8dc6"/>
+    <ds:schemaRef ds:uri="d173ed03-a843-4ceb-a512-f7ef0c28f5c6"/>
+    <ds:schemaRef ds:uri="a059ad7d-a67f-441f-a04d-fea35a8d4805"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>